<commit_message>
added error bars for x data
</commit_message>
<xml_diff>
--- a/jupyter/lab6/rawData/measurements.xlsx
+++ b/jupyter/lab6/rawData/measurements.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>deltah(cm)</t>
   </si>
@@ -229,7 +229,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -312,7 +311,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Part1!$B$1:$B$17</c:f>
+              <c:f>Part1!$C$1:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -381,11 +380,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="97298720"/>
-        <c:axId val="23501776"/>
+        <c:axId val="-540907088"/>
+        <c:axId val="-647397632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97298720"/>
+        <c:axId val="-540907088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,7 +406,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -424,7 +422,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23501776"/>
+        <c:crossAx val="-647397632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -432,7 +430,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23501776"/>
+        <c:axId val="-647397632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,14 +464,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97298720"/>
+        <c:crossAx val="-540907088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1985,35 +1982,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2024,312 +2027,408 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <v>-75</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
         <v>-270</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>-5</v>
       </c>
       <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>-17</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
       <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <v>-70</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
         <v>-255</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>-10</v>
       </c>
       <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>-34</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
       <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
         <v>-65</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
         <v>-239</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>-15</v>
       </c>
       <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>-54</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
       <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
         <v>-60</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
         <v>-222</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>-20</v>
       </c>
       <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>-67</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
       <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>-55</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
         <v>-206</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>-25</v>
       </c>
       <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>-86</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
       <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
         <v>-50</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
         <v>-189</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>-30</v>
       </c>
       <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
         <v>-106</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
       <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
         <v>-45</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
         <v>-171</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>-35</v>
       </c>
       <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <v>-122</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
       <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
         <v>-40</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
         <v>-155</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>-40</v>
       </c>
       <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>-141</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
       <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
         <v>-35</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
         <v>-136</v>
       </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>-45</v>
       </c>
       <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
         <v>-160</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
       <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
         <v>-30</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
         <v>-119</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>-50</v>
       </c>
       <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>-177</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
       <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>-25</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
         <v>-102</v>
       </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>-55</v>
       </c>
       <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
         <v>-194</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
       <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
         <v>-20</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
         <v>-84</v>
       </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>-60</v>
       </c>
       <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
         <v>-213</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
       <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
         <v>-15</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
         <v>-66</v>
       </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>-65</v>
       </c>
       <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
         <v>-232</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
       <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
         <v>-10</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
         <v>-48</v>
       </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>-70</v>
       </c>
       <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
         <v>-251</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
       <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
         <v>-5</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
         <v>-32</v>
       </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>-75</v>
       </c>
       <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
         <v>-270</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
       <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
         <v>-15</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>